<commit_message>
actualización del archivo traza.xlsx para el ejercicio 6
</commit_message>
<xml_diff>
--- a/TP4/ej6/traza.xlsx
+++ b/TP4/ej6/traza.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Codigos\Algoritmica-Programacion-II\TP4\ej6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Facultad\AyP2\codigos\TP4\ej6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{26E26048-B2EF-43B6-B921-E3BD0AC92A35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A09057D3-2539-46F4-A365-1CD0147635BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E682BA14-EF0F-4893-AB68-E920073F7E5F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E682BA14-EF0F-4893-AB68-E920073F7E5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>numbers []</t>
   </si>
@@ -48,6 +48,48 @@
   </si>
   <si>
     <t>quicksort(int low, int high)</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pivot</t>
+  </si>
+  <si>
+    <t>while(i&lt;=j)</t>
+  </si>
+  <si>
+    <t>while(numbers[i]&lt;pivot)</t>
+  </si>
+  <si>
+    <t>i++</t>
+  </si>
+  <si>
+    <t>while(numbers[j] &gt;pivot)</t>
+  </si>
+  <si>
+    <t>j--</t>
+  </si>
+  <si>
+    <t>i &lt;=j</t>
+  </si>
+  <si>
+    <t>exchange(i,j)</t>
+  </si>
+  <si>
+    <t>low &lt; j</t>
+  </si>
+  <si>
+    <t>quicksort(low, j)</t>
+  </si>
+  <si>
+    <t>quicksort( I, high)</t>
+  </si>
+  <si>
+    <t>I &lt; high</t>
   </si>
 </sst>
 </file>
@@ -115,7 +157,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -431,31 +473,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33190313-CBB1-467D-9789-4EA0DD9FFA76}">
-  <dimension ref="B5:D6"/>
+  <dimension ref="B5:R6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="34.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" style="2" customWidth="1"/>
+    <col min="4" max="4" width="34.140625" style="2" customWidth="1"/>
+    <col min="5" max="8" width="11.42578125" style="2"/>
+    <col min="9" max="9" width="23.28515625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="2"/>
+    <col min="11" max="11" width="23.140625" style="2" customWidth="1"/>
+    <col min="12" max="13" width="11.42578125" style="2"/>
+    <col min="14" max="14" width="16" style="2" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" style="2"/>
+    <col min="16" max="16" width="18" style="2" customWidth="1"/>
+    <col min="17" max="17" width="18.28515625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="22.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="6" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>

</xml_diff>